<commit_message>
atualizações na coluna existentes  planilha BMA
</commit_message>
<xml_diff>
--- a/Necessidades da OMs.xlsx
+++ b/Necessidades da OMs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitorvhfca\Nextcloud\DTTO\vitor\Python\Tesserato2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55602A19-E1C2-454C-89A1-1EEE6D6010DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016153B7-497B-4547-A3A1-E6A68837B183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C0D63444-7A24-48F2-AA92-03F9F05044A0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C0D63444-7A24-48F2-AA92-03F9F05044A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessidades" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -826,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA977D7E-CCF4-482E-AC09-3059058AA1AA}">
   <dimension ref="A2:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,4 +1509,60 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97524A1-D21A-4D81-A9F7-C432AD6437A7}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f ca="1">RANDBETWEEN(0, $B$1)</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f ca="1">SMALL($A$4:$A$6, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f ca="1">RANDBETWEEN(0, $B$1)</f>
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f ca="1">SMALL($A$4:$A$6, 2) - SMALL($A$4:$A$6, 1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f ca="1">RANDBETWEEN(0, $B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f ca="1">SMALL($A$4:$A$6, 3) - SMALL($A$4:$A$6, 2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f ca="1">$B$1 - SMALL($A$4:$A$6, 3)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>